<commit_message>
Change rede 3 classes; Upd reports
</commit_message>
<xml_diff>
--- a/reports/semiauto_class_distributions.xlsx
+++ b/reports/semiauto_class_distributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto Final\Projeto Petrobras\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740D2A1-E8CB-4A96-840E-47FEF0AA3B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DB9029-7196-4CB7-82D9-2ADD26400869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
   <si>
     <t>Manual</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Sem pesos</t>
   </si>
   <si>
-    <t>Com pesos</t>
-  </si>
-  <si>
     <t>Diff Automatic - Manual</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>Enterramento</t>
+  </si>
+  <si>
+    <t>Com pesos (acho que é igual)</t>
+  </si>
+  <si>
+    <t>obs: enterramento foi anotado só com pesos na vdd</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -339,22 +342,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -385,6 +377,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -409,16 +410,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:R23"/>
+  <dimension ref="A3:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,34 +709,34 @@
         <v>12</v>
       </c>
       <c r="M3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="26" t="s">
+      <c r="C4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="M4" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="26" t="s">
+      <c r="H4" s="32"/>
+      <c r="M4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="29"/>
+      <c r="O4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="29"/>
+      <c r="R4" s="32"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
@@ -764,7 +758,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>11</v>
@@ -786,7 +780,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -819,9 +813,9 @@
         <v>3.0765086669152203E-2</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="22" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -847,7 +841,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
@@ -873,7 +867,7 @@
         <f>G7/G$8</f>
         <v>0.956803935692501</v>
       </c>
-      <c r="K7" s="31"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
@@ -897,7 +891,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
@@ -918,14 +912,14 @@
         <v>1</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" ref="G8:G20" si="1">C8+E8</f>
+        <f t="shared" ref="G8:G23" si="1">C8+E8</f>
         <v>130498</v>
       </c>
       <c r="H8" s="17">
         <f>G8/G$8</f>
         <v>1</v>
       </c>
-      <c r="K8" s="31"/>
+      <c r="K8" s="23"/>
       <c r="L8" s="5" t="s">
         <v>4</v>
       </c>
@@ -955,7 +949,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -988,9 +982,9 @@
         <v>0.11605616266540238</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -1016,7 +1010,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1036,7 @@
         <f>G10/G$11</f>
         <v>0.99105328927698</v>
       </c>
-      <c r="K10" s="31"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1060,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1088,7 @@
         <f>G11/G$11</f>
         <v>1</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1124,7 +1118,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1157,9 +1151,9 @@
         <v>0.26669531662415558</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="23" t="s">
         <v>7</v>
       </c>
       <c r="L12" s="5" t="s">
@@ -1185,7 +1179,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1211,7 +1205,7 @@
         <f>G13/G$14</f>
         <v>0.83938272456305696</v>
       </c>
-      <c r="K13" s="31"/>
+      <c r="K13" s="23"/>
       <c r="L13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1229,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +1257,7 @@
         <f>G14/G$14</f>
         <v>1</v>
       </c>
-      <c r="K14" s="31"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1284,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1323,9 +1317,9 @@
         <v>0.24805868053601665</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="4" t="s">
@@ -1351,7 +1345,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1371,7 @@
         <f t="shared" si="4"/>
         <v>0.89585872289544477</v>
       </c>
-      <c r="K16" s="31"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="5" t="s">
         <v>3</v>
       </c>
@@ -1401,7 +1395,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1429,7 +1423,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1453,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1492,9 +1486,9 @@
         <v>0.74578678005320553</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="23" t="s">
         <v>9</v>
       </c>
       <c r="L18" s="5" t="s">
@@ -1524,7 +1518,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1544,7 @@
         <f t="shared" si="4"/>
         <v>0.14821372454337112</v>
       </c>
-      <c r="K19" s="31"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1578,7 +1572,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1606,7 +1600,7 @@
         <f t="shared" si="4"/>
         <v>0.99708738608230429</v>
       </c>
-      <c r="K20" s="32"/>
+      <c r="K20" s="24"/>
       <c r="L20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1636,98 +1630,199 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G21" s="1"/>
-      <c r="K21" s="30" t="s">
-        <v>19</v>
+      <c r="A21" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="18">
+        <v>5501</v>
+      </c>
+      <c r="D21" s="33">
+        <f>C21/C$23</f>
+        <v>0.62976531196336571</v>
+      </c>
+      <c r="E21" s="1">
+        <v>37339</v>
+      </c>
+      <c r="F21" s="33">
+        <f>E21/E$23</f>
+        <v>0.3080318104571928</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>42840</v>
+      </c>
+      <c r="H21" s="15">
+        <f>G21/G$23</f>
+        <v>0.32965764545643422</v>
+      </c>
+      <c r="I21" s="20">
+        <f>ABS(D21-F21)</f>
+        <v>0.32173350150617291</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="12" t="e">
-        <f t="shared" ref="N21:N23" si="5">M21/M$17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" s="8"/>
-      <c r="P21" s="12" t="e">
-        <f t="shared" ref="P21:P23" si="6">O21/O$17</f>
-        <v>#DIV/0!</v>
+      <c r="M21" s="18">
+        <v>5501</v>
+      </c>
+      <c r="N21" s="33">
+        <f>M21/M$23</f>
+        <v>0.62976531196336571</v>
+      </c>
+      <c r="O21" s="1">
+        <v>37339</v>
+      </c>
+      <c r="P21" s="33">
+        <f>O21/O$23</f>
+        <v>0.3080318104571928</v>
       </c>
       <c r="Q21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="15" t="e">
-        <f t="shared" ref="R21:R23" si="7">Q21/Q$17</f>
-        <v>#DIV/0!</v>
+        <v>42840</v>
+      </c>
+      <c r="R21" s="15">
+        <f>Q21/Q$23</f>
+        <v>0.32965764545643422</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K22" s="31"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="18">
+        <v>3234</v>
+      </c>
+      <c r="D22" s="34">
+        <f t="shared" ref="D22:D23" si="5">C22/C$23</f>
+        <v>0.37023468803663423</v>
+      </c>
+      <c r="E22" s="2">
+        <v>83879</v>
+      </c>
+      <c r="F22" s="34">
+        <f t="shared" ref="F22:F23" si="6">E22/E$23</f>
+        <v>0.69196818954280714</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>87113</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" ref="H22:H23" si="7">G22/G$23</f>
+        <v>0.67034235454356572</v>
+      </c>
+      <c r="K22" s="23"/>
       <c r="L22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="13" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="13" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+      <c r="M22" s="18">
+        <v>3234</v>
+      </c>
+      <c r="N22" s="34">
+        <f t="shared" ref="N22:N23" si="8">M22/M$23</f>
+        <v>0.37023468803663423</v>
+      </c>
+      <c r="O22" s="2">
+        <v>83879</v>
+      </c>
+      <c r="P22" s="34">
+        <f t="shared" ref="P22:P23" si="9">O22/O$23</f>
+        <v>0.69196818954280714</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="16" t="e">
+        <v>87113</v>
+      </c>
+      <c r="R22" s="16">
+        <f t="shared" ref="R22:R23" si="10">Q22/Q$23</f>
+        <v>0.67034235454356572</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <f>C21+C22</f>
+        <v>8735</v>
+      </c>
+      <c r="D23" s="35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <f>E21+E22</f>
+        <v>121218</v>
+      </c>
+      <c r="F23" s="35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="1"/>
+        <v>129953</v>
+      </c>
+      <c r="H23" s="17">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K23" s="32"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="24"/>
       <c r="L23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="M23" s="3">
         <f>M21+M22</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="14" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>8735</v>
+      </c>
+      <c r="N23" s="35">
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="O23" s="3">
         <f>O21+O22</f>
-        <v>0</v>
-      </c>
-      <c r="P23" s="14" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q23" s="33">
+        <v>121218</v>
+      </c>
+      <c r="P23" s="35">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="17" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>129953</v>
+      </c>
+      <c r="R23" s="17">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="K15:K17"/>
     <mergeCell ref="K21:K23"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="K15:K17"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
@@ -1735,6 +1830,7 @@
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>